<commit_message>
updated requirements to shall
</commit_message>
<xml_diff>
--- a/scheme/tools/Conformity-Assessment-Workbook.xlsx
+++ b/scheme/tools/Conformity-Assessment-Workbook.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" state="visible" r:id="rId2"/>
@@ -890,7 +890,7 @@
     <t xml:space="preserve">4.1.1.1</t>
   </si>
   <si>
-    <t xml:space="preserve">Where an Organization will issue and/or consume Identity and/or Credentials as part of its identity context, including as part of a federation, the Organization shall define and implement criteria for selecting a trust framework 1 that will
+    <t xml:space="preserve">Where an Organization will issue and/or consume Identity and/or Credentials as part of its identity context, including as part of a federation, the Organization SHALL define and implement criteria for selecting a trust framework 1 that will
 govern the operation of its identity management system and the rights and obligations of the federation participants, so as to ensure the trustworthiness of its identity management system and those of the federation participants. Organizations should consider the following when defining criteria for selecting a trust framework:
 a. the Organization’s context including its contractual obligations;
 b. the industry sector in which the Organization operates including
@@ -918,25 +918,25 @@
     <t xml:space="preserve">4.2.1.1</t>
   </si>
   <si>
-    <t xml:space="preserve">The Organization shall, absent legal directives, select Identity attributes to distinguish a unique Identity that meet the Organization’s needs and requirements, in a manner that balances risk, flexibility, and inclusiveness.</t>
+    <t xml:space="preserve">The Organization SHALL, absent legal directives, select Identity attributes to distinguish a unique Identity that meet the Organization’s needs and requirements, in a manner that balances risk, flexibility, and inclusiveness.</t>
   </si>
   <si>
     <t xml:space="preserve">4.2.1.2</t>
   </si>
   <si>
-    <t xml:space="preserve">The Organization shall evaluate Identity Verification risks and/or Credential Verification risks by assessing potential impacts to a Person, an activity, a service, a transaction, or a sector.</t>
+    <t xml:space="preserve">The Organization SHALL evaluate Identity Verification risks and/or Credential Verification risks by assessing potential impacts to a Person, an activity, a service, a transaction, or a sector.</t>
   </si>
   <si>
     <t xml:space="preserve">4.2.1.3</t>
   </si>
   <si>
-    <t xml:space="preserve">The Organization shall, with respect to Identity and Credential processes, apply the required Identity assurance levels and/or credential assurance levels and related controls for achieving assurance level requirements.</t>
+    <t xml:space="preserve">The Organization SHALL, with respect to Identity and Credential processes, apply the required Identity assurance levels and/or credential assurance levels and related controls for achieving assurance level requirements.</t>
   </si>
   <si>
     <t xml:space="preserve">4.2.1.4</t>
   </si>
   <si>
-    <t xml:space="preserve">The Organization shall monitor its identity management systems and processes to ensure their availability, integrity, and confidentiality, and shall evaluate the federation’s trust framework for the same purpose.</t>
+    <t xml:space="preserve">The Organization SHALL monitor its identity management systems and processes to ensure their availability, integrity, and confidentiality, and shall evaluate the federation’s trust framework for the same purpose.</t>
   </si>
   <si>
     <t xml:space="preserve">Leadership</t>
@@ -948,7 +948,7 @@
     <t xml:space="preserve">5.1.1.1</t>
   </si>
   <si>
-    <t xml:space="preserve">Top management shall demonstrate their commitment to the Organization’s Digital Identity systems and services by:</t>
+    <t xml:space="preserve">Top management SHALL demonstrate their commitment to the Organization’s Digital Identity systems and services by:</t>
   </si>
   <si>
     <t xml:space="preserve">5.1.1.1.a</t>
@@ -994,7 +994,7 @@
     <t xml:space="preserve">6.1.1.1</t>
   </si>
   <si>
-    <t xml:space="preserve">When planning for the Organization’s Digital Identity systems and services, the Organization shall consider the issues and requirements outlined in Section 4, and determine the risks and opportunities that need to be addressed to:
+    <t xml:space="preserve">When planning for the Organization’s Digital Identity systems and services, the Organization SHALL consider the issues and requirements outlined in Section 4, and determine the risks and opportunities that need to be addressed to:
 • give assurance that the Digital Identity systems and services can
 achieve their intended result(s);
 • prevent, or reduce, undesired effects; and
@@ -1004,7 +1004,7 @@
     <t xml:space="preserve">6.1.1.2</t>
   </si>
   <si>
-    <t xml:space="preserve">The Organization shall plan:
+    <t xml:space="preserve">The Organization SHALL plan:
 a. actions to address these risks and opportunities; and
 b. how to:
 integrate and implement the actions into its Digital Identity
@@ -1018,13 +1018,13 @@
     <t xml:space="preserve">6.2.1.1</t>
   </si>
   <si>
-    <t xml:space="preserve">The Organization shall establish objectives for its Digital Identity systems and services.</t>
+    <t xml:space="preserve">The Organization SHALL establish objectives for its Digital Identity systems and services.</t>
   </si>
   <si>
     <t xml:space="preserve">6.2.1.2</t>
   </si>
   <si>
-    <t xml:space="preserve">These objectives shall:
+    <t xml:space="preserve">These objectives SHALL:
 a. be consistent with the existing policies;
 b. be measurable (if practicable);
 c. take into account applicable requirements;
@@ -1037,7 +1037,7 @@
     <t xml:space="preserve">6.2.1.3</t>
   </si>
   <si>
-    <t xml:space="preserve">When planning how to achieve these objectives, the Organization shall
+    <t xml:space="preserve">When planning how to achieve these objectives, the Organization SHALL
 determine:
 • what will be done;
 • what resources will be required;
@@ -1052,7 +1052,7 @@
     <t xml:space="preserve">6.3.1.1</t>
   </si>
   <si>
-    <t xml:space="preserve">When the Organization determines the need for changes to its Digital Identity systems and services, the changes shall be carried out in a planned manner.</t>
+    <t xml:space="preserve">When the Organization determines the need for changes to its Digital Identity systems and services, the changes SHALL be carried out in a planned manner.</t>
   </si>
   <si>
     <t xml:space="preserve">Support</t>
@@ -1064,7 +1064,7 @@
     <t xml:space="preserve">7.1.1.1</t>
   </si>
   <si>
-    <t xml:space="preserve">The Organization shall determine the resources needed for the establishment, implementation, maintenance, and continual improvement of Digital Identity systems and services.</t>
+    <t xml:space="preserve">The Organization SHALL determine the resources needed for the establishment, implementation, maintenance, and continual improvement of Digital Identity systems and services.</t>
   </si>
   <si>
     <t xml:space="preserve">Competence</t>
@@ -1073,19 +1073,19 @@
     <t xml:space="preserve">7.2.1.1</t>
   </si>
   <si>
-    <t xml:space="preserve">The Organization shall determine the necessary competence of person(s) doing work that affects the performance of Digital Identity systems and services.</t>
+    <t xml:space="preserve">The Organization SHALL determine the necessary competence of person(s) doing work that affects the performance of Digital Identity systems and services.</t>
   </si>
   <si>
     <t xml:space="preserve">7.2.1.2</t>
   </si>
   <si>
-    <t xml:space="preserve">The Organization shall ensure that the persons contemplated in 7.2.1.1 are competent on the basis of appropriate education, training, and experience.</t>
+    <t xml:space="preserve">The Organization SHALL ensure that the persons contemplated in 7.2.1.1 are competent on the basis of appropriate education, training, and experience.</t>
   </si>
   <si>
     <t xml:space="preserve">7.2.1.3</t>
   </si>
   <si>
-    <t xml:space="preserve">The Organization shall, where applicable, take actions to acquire the necessary competence, and evaluate the effectiveness of the actions taken.</t>
+    <t xml:space="preserve">The Organization SHALL, where applicable, take actions to acquire the necessary competence, and evaluate the effectiveness of the actions taken.</t>
   </si>
   <si>
     <t xml:space="preserve">Awareness</t>
@@ -1094,7 +1094,7 @@
     <t xml:space="preserve">7.3.1.1</t>
   </si>
   <si>
-    <t xml:space="preserve">To ensure the successful implementation required by the Outcomes listed in Section 8, persons doing work related to Digital Identity systems and services shall be aware of:
+    <t xml:space="preserve">To ensure the successful implementation required by the Outcomes listed in Section 8, persons doing work related to Digital Identity systems and services SHALL be aware of:
 • All manual and automated controls;
 • All policies and procedures that they must follow; and
 • The implications of not conforming to the requirements of this document, particularly the implications on the subjects of the Digital Identity systems and services.</t>
@@ -1184,7 +1184,7 @@
     <t xml:space="preserve">GEN</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST ensure that policies and plans are developed, documented, and disseminated within the organization that address at the enterprise level: 
+    <t xml:space="preserve">The entity under assessment SHALL ensure that policies and plans are developed, documented, and disseminated within the organization that address at the enterprise level: 
   ● Risk assessment; 
   ● Audit and accountability; 
   ● Security assessment; 
@@ -1202,14 +1202,14 @@
     <t xml:space="preserve">ENWM.02</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST ensure that the formal operational policy and procedures, identified in ENWM.01, are reviewed and updated regularly on a fixed schedule appropriate to the context of the program/service being delivered. 
+    <t xml:space="preserve">The entity under assessment SHALL ensure that the formal operational policy and procedures, identified in ENWM.01, are reviewed and updated regularly on a fixed schedule appropriate to the context of the program/service being delivered. 
 Policies/plans may also require update on an ad hoc basis based on operational events or extraordinary need.</t>
   </si>
   <si>
     <t xml:space="preserve">ENWM.03</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST have active procedures that reflect the operational policy requirements for:
+    <t xml:space="preserve">The entity under assessment SHALL have active procedures that reflect the operational policy requirements for:
   ● provision of notice,
   ● activity audit,
   ● information maintenance
@@ -1221,13 +1221,13 @@
     <t xml:space="preserve">ENWM.04</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST specify its mandate and authority as these relate to the identification of entities and to the relationships between entities.</t>
+    <t xml:space="preserve">The entity under assessment SHALL specify its mandate and authority as these relate to the identification of entities and to the relationships between entities.</t>
   </si>
   <si>
     <t xml:space="preserve">ENWM.05</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST provide a description of the program or service, including:
+    <t xml:space="preserve">The entity under assessment SHALL provide a description of the program or service, including:
 1. The type and nature of the program or service;
 2. The intended clients of the program or service; AND
 3. The approximate size, characteristics, and composition of the client population.</t>
@@ -1236,19 +1236,19 @@
     <t xml:space="preserve">ENWM.06</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST ensure that personal information, organizational information, and relationship information are collected and managed under relevant law, regulation, and policy.</t>
+    <t xml:space="preserve">The entity under assessment SHALL ensure that personal information, organizational information, and relationship information are collected and managed under relevant law, regulation, and policy.</t>
   </si>
   <si>
     <t xml:space="preserve">ENWM.07</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST identify the authorized operational roles, access management processes, and modification processes pertaining to the collection and management of information.</t>
+    <t xml:space="preserve">The entity under assessment SHALL identify the authorized operational roles, access management processes, and modification processes pertaining to the collection and management of information.</t>
   </si>
   <si>
     <t xml:space="preserve">ENWM.08</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST have quality assurance processes (e.g., monitoring, measurement) in place to ensure consistent execution of operational tasks. 
+    <t xml:space="preserve">The entity under assessment SHALL have quality assurance processes (e.g., monitoring, measurement) in place to ensure consistent execution of operational tasks. 
 Specifically, this pertains to operational activities such as:
   ● front counter activities; 
   ● back office activities such as information processing and adjudication; and, 
@@ -1258,13 +1258,13 @@
     <t xml:space="preserve">ENWM.09</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST provide notice to entities providing identity evidence or relationship evidence that false or misleading statements may result in violation of the terms and conditions of the program or service.</t>
+    <t xml:space="preserve">The entity under assessment SHALL provide notice to entities providing identity evidence or relationship evidence that false or misleading statements may result in violation of the terms and conditions of the program or service.</t>
   </si>
   <si>
     <t xml:space="preserve">ENWM.10</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MAY rely on another entity to carry out program or service activities that are subject to these conformance criteria. In such cases, the entity under assessment MUST:
+    <t xml:space="preserve">The entity under assessment MAY rely on another entity to carry out program or service activities that are subject to these conformance criteria. In such cases, the entity under assessment SHALL:
 1. Provide documentation of the written agreement for the arrangement in effect; AND
 2. Provide documentation of the agreed upon conformance criteria.</t>
   </si>
@@ -1272,37 +1272,37 @@
     <t xml:space="preserve">ENWM.11</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST ensure that service providers to whom they have delegated service provision tasks adhere to applicable conformance criteria.</t>
+    <t xml:space="preserve">The entity under assessment SHALL ensure that service providers to whom they have delegated service provision tasks adhere to applicable conformance criteria.</t>
   </si>
   <si>
     <t xml:space="preserve">ENWM.12</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST manage system components using its defined system development life cycle that incorporates security concerns.</t>
+    <t xml:space="preserve">The entity under assessment SHALL manage system components using its defined system development life cycle that incorporates security concerns.</t>
   </si>
   <si>
     <t xml:space="preserve">ENWM.13</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST have formal technology change management processes in place to evaluate and manage risk associated with technology evolution.</t>
+    <t xml:space="preserve">The entity under assessment SHALL have formal technology change management processes in place to evaluate and manage risk associated with technology evolution.</t>
   </si>
   <si>
     <t xml:space="preserve">ENWM.14</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST ensure that its personnel responsible for operations affecting personal information, organizational information, and relationship information have received privacy and security training.</t>
+    <t xml:space="preserve">The entity under assessment SHALL ensure that its personnel responsible for operations affecting personal information, organizational information, and relationship information have received privacy and security training.</t>
   </si>
   <si>
     <t xml:space="preserve">ENWM.15</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST uniquely identify and authenticate non-organizational personnel or users, or processes acting on behalf of non-organizational personnnel or users, where authentication is appropriate.</t>
+    <t xml:space="preserve">The entity under assessment SHALL uniquely identify and authenticate non-organizational personnel or users, or processes acting on behalf of non-organizational personnnel or users, where authentication is appropriate.</t>
   </si>
   <si>
     <t xml:space="preserve">ENWM.16</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST enforce access controls to ensure that only authorized personnel can update identity information or relationship information.</t>
+    <t xml:space="preserve">The entity under assessment SHALL enforce access controls to ensure that only authorized personnel can update identity information or relationship information.</t>
   </si>
   <si>
     <t xml:space="preserve">IDDG</t>
@@ -1462,19 +1462,19 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST adhere to applicable identity management controls, standards, and guidelines, and MUST have an auditable process to demonstrate adherence.</t>
+    <t xml:space="preserve">The entity under assessment SHALL adhere to applicable identity management controls, standards, and guidelines, and SHALL have an auditable process to demonstrate adherence.</t>
   </si>
   <si>
     <t xml:space="preserve">IDDG.03</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST provide a list of the applicable identity management controls, standards, and guidelines that are in effect.</t>
+    <t xml:space="preserve">The entity under assessment SHALL provide a list of the applicable identity management controls, standards, and guidelines that are in effect.</t>
   </si>
   <si>
     <t xml:space="preserve">IDDG.04</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST demonstrate the equivalency of the applicable identity management controls, standards, and guidelines to those used by the assessor. </t>
+    <t xml:space="preserve">The entity under assessment SHALL demonstrate the equivalency of the applicable identity management controls, standards, and guidelines to those used by the assessor. </t>
   </si>
   <si>
     <t xml:space="preserve">IDDG.05</t>
@@ -1514,13 +1514,13 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST have in place policies and procedures to safeguard the identity information of a person.</t>
+    <t xml:space="preserve">The entity under assessment SHALL have in place policies and procedures to safeguard the identity information of a person.</t>
   </si>
   <si>
     <t xml:space="preserve">IDDG.06</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST have in place policies and procedures to detect the misuse of the identity information of a person.</t>
+    <t xml:space="preserve">The entity under assessment SHALL have in place policies and procedures to detect the misuse of the identity information of a person.</t>
   </si>
   <si>
     <t xml:space="preserve">IDDG.07</t>
@@ -1600,7 +1600,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST ensure that identity information validation of acceptable information providers who are persons, meets or exceeds the requirements applicable to the IP2 (for persons) qualifier in Identity Information Validation.</t>
+    <t xml:space="preserve">The entity under assessment SHALL ensure that identity information validation of acceptable information providers who are persons, meets or exceeds the requirements applicable to the IP2 (for persons) qualifier in Identity Information Validation.</t>
   </si>
   <si>
     <t xml:space="preserve">IDDG.09</t>
@@ -1640,19 +1640,19 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST ensure that identity information validation of acceptable information providers who are persons, meets the requirements applicable to the IP3 (for persons) qualifier in Identity Information Validation.</t>
+    <t xml:space="preserve">The entity under assessment SHALL ensure that identity information validation of acceptable information providers who are persons, meets the requirements applicable to the IP3 (for persons) qualifier in Identity Information Validation.</t>
   </si>
   <si>
     <t xml:space="preserve">IDDG.10</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST ensure that identity verification of acceptable information providers who are persons, meets the requirements applicable to the IP3 (for persons) qualifier in Identity Verification.</t>
+    <t xml:space="preserve">The entity under assessment SHALL ensure that identity verification of acceptable information providers who are persons, meets the requirements applicable to the IP3 (for persons) qualifier in Identity Verification.</t>
   </si>
   <si>
     <t xml:space="preserve">IDDG.11</t>
   </si>
   <si>
-    <t xml:space="preserve">In cases involving children, minors, and other vulnerable individuals, the entity under assessment MUST:    
+    <t xml:space="preserve">In cases involving children, minors, and other vulnerable individuals, the entity under assessment SHALL:    
 1. Have in place additional safeguards, compensating factors, or a documented exception process to reduce risk and to initiate interventions, as appropriate; AND
 2. Confirm that the applicant (for example, a parent or guardian) has the legal authority to carry out a request or obtain a service on behalf of the child, minor, or other vulnerable individual.</t>
   </si>
@@ -1749,7 +1749,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST specify the identity context of the program or service.
+    <t xml:space="preserve">The entity under assessment SHALL specify the identity context of the program or service.
 The following considerations should be kept in mind when defining the identity context of a program or service: 
   ● Intended recipients of the program or service – recipients may be external to the program/service provider (e.g., citizens, businesses, non-profit organizations), or internal to the program/service provider (e.g., employees, departments)
   ● Size, characteristics, and composition of the client population
@@ -1758,13 +1758,13 @@
   ● Use of shared services where the shared service delivery context may differ from the program context</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST define the identity information requirements of the program or service.
+    <t xml:space="preserve">The entity under assessment SHALL define the identity information requirements of the program or service.
 For any given program or service, identity information is the set of identity attributes that is both:
   ● Sufficient to distinguish between different entities within the program/service population (i.e., achieve the uniqueness requirement for identity); and
   ● Sufficient to describe the entity as required by the program or service.</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST define the set of identity attributes that will be used to uniquely distinguish a particular entity within the program/service population. This set of identity attributes is referred to as the identifier.</t>
+    <t xml:space="preserve">The entity under assessment SHALL define the set of identity attributes that will be used to uniquely distinguish a particular entity within the program/service population. This set of identity attributes is referred to as the identifier.</t>
   </si>
   <si>
     <t xml:space="preserve">IDED</t>
@@ -1840,8 +1840,8 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST determine the acceptable evidence of foundational identity (whether physical or electronic) for its programs and services.
-The entity under assessment MUST ensure that the evidence of foundational identity originates from an authoritative source that:
+    <t xml:space="preserve">The entity under assessment SHALL determine the acceptable evidence of foundational identity (whether physical or electronic) for its programs and services.
+The entity under assessment SHALL ensure that the evidence of foundational identity originates from an authoritative source that:
 1. Is under the control of a federal, provincial, or territorial government, or the local equivalent abroad (Note: When the authoritative source is outside Canadian jurisdiction, the acceptability criteria will be determined through a risk-managed approach); and
 2. Registers specific foundational events, or determines legal status.
 Acceptable authoritative records and credentials are:
@@ -1854,47 +1854,18 @@
     <t xml:space="preserve">IDED.02</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">The entity under assessment MUST determine the acceptable evidence of contextual identity (whether physical or electronic)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">for it programs and services.  
-The entity under assessment MUST ensure that the evidence of contextual identity originates from an authoritative source that is under the control of an organization that has been approved by the entity under assessment.
+    <t xml:space="preserve">The entity under assessment SHALL determine the acceptable evidence of contextual identity (whether physical or electronic) for it programs and services.  
+The entity under assessment SHALL ensure that the evidence of contextual identity originates from an authoritative source that is under the control of an organization that has been approved by the entity under assessment.
 Some examples of acceptable authoritative records and credentials are:
  ● Licensing and registration records used in the issuance of a health insurance card or a driver's licence;
  ● Records of professional qualifications used in the issuance of professional credentials; and
  ● Membership records used in the issuance of membership credentials.</t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">IDED.03</t>
   </si>
   <si>
-    <t xml:space="preserve">When assessing authoritative souces of evidence of contextual identity (whether physical or electronic), the entity under assessment MUST take the following into consideration: 
+    <t xml:space="preserve">When assessing authoritative souces of evidence of contextual identity (whether physical or electronic), the entity under assessment SHALL take the following into consideration: 
 1. The recognition of the authoritative source in law;
 2. The ability of the authoritative source to satisfy relevant regulatory authorities;
 3. The historic performance of the authoritative source;
@@ -1911,7 +1882,7 @@
     <t xml:space="preserve">IDED.05</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST identify the acceptable information providers from which evidence of contextual or foundational identity will be accepted.</t>
+    <t xml:space="preserve">The entity under assessment SHALL identify the acceptable information providers from which evidence of contextual or foundational identity will be accepted.</t>
   </si>
   <si>
     <t xml:space="preserve">IDEA</t>
@@ -1987,13 +1958,13 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST ensure that the entities presenting evidence of contextual or foundational identity are acceptable information providers as defined in Identity Evidence Determination.  </t>
+    <t xml:space="preserve">The entity under assessment SHALL ensure that the entities presenting evidence of contextual or foundational identity are acceptable information providers as defined in Identity Evidence Determination.  </t>
   </si>
   <si>
     <t xml:space="preserve">IDEA.02</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST NOT restrict what is provided as evidence of identity.</t>
+    <t xml:space="preserve">The entity under assessment SHALL NOT restrict what is provided as evidence of identity.</t>
   </si>
   <si>
     <t xml:space="preserve">IDEA.03</t>
@@ -2033,7 +2004,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST require that one instance of evidence of identity (either foundational or contextual) be provided.</t>
+    <t xml:space="preserve">The entity under assessment SHALL require that one instance of evidence of identity (either foundational or contextual) be provided.</t>
   </si>
   <si>
     <t xml:space="preserve">IDEA.04</t>
@@ -2073,7 +2044,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST require that two instances of evidence of identity (at least one of which must be evidence of foundational identity) be provided.</t>
+    <t xml:space="preserve">The entity under assessment SHALL require that two instances of evidence of identity (at least one of which SHALL be evidence of foundational identity) be provided.</t>
   </si>
   <si>
     <t xml:space="preserve">IDEA.05</t>
@@ -2095,7 +2066,7 @@
     <t xml:space="preserve">IP3</t>
   </si>
   <si>
-    <t xml:space="preserve">In cases involving children, minors, and other vulnerable individuals, the entity under assessment MUST require evidence of identity of the applicant (for example, a parent or guardian) in addition to evidence of identity of the child, minor, or other vulnerable individual. For example, the passport of a parent could be used as evidence of contextual identity of the child.</t>
+    <t xml:space="preserve">In cases involving children, minors, and other vulnerable individuals, the entity under assessment SHALL require evidence of identity of the applicant (for example, a parent or guardian) in addition to evidence of identity of the child, minor, or other vulnerable individual. For example, the passport of a parent could be used as evidence of contextual identity of the child.</t>
   </si>
   <si>
     <t xml:space="preserve">IDIV</t>
@@ -2184,27 +2155,27 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST ensure that the evidence of identity has a defined validity period.</t>
+    <t xml:space="preserve">The entity under assessment SHALL ensure that the evidence of identity has a defined validity period.</t>
   </si>
   <si>
     <t xml:space="preserve">IDIV.04</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST ensure that assertions of identity information made by an entity about a Subject acceptably match all instances of evidence of identity (foundational and/or contextual) provided by the Holder.</t>
+    <t xml:space="preserve">The entity under assessment SHALL ensure that assertions of identity information made by an entity about a Subject acceptably match all instances of evidence of identity (foundational and/or contextual) provided by the Holder.</t>
   </si>
   <si>
     <t xml:space="preserve">IDIV.05</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST confirm the the evidence of contextual identity with the issuing authority AND MUST validate the identity information against the authoritative record AND SHOULD request the status of the Subject from the issuing authority.
-If confirmation with the issuing authority or validation of the identity information is not feasible, then the entity under assessment MUST ensure that the evidence of contextual identity is confirmed by a trained examiner.</t>
+    <t xml:space="preserve">The entity under assessment SHALL confirm the the evidence of contextual identity with the issuing authority AND SHALL validate the identity information against the authoritative record AND SHOULD request the status of the Subject from the issuing authority.
+If confirmation with the issuing authority or validation of the identity information is not feasible, then the entity under assessment SHALL ensure that the evidence of contextual identity is confirmed by a trained examiner.</t>
   </si>
   <si>
     <t xml:space="preserve">IDIV.06</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST confirm the the evidence of foundational identity with the issuing authority AND MUST validate the identity information against the authoritative record AND MUST request the status of the Subject from the issuing authority.
-If confirmation with the issuing authority or validation of the identity information is not feasible, then the entity under assessment MUST ensure that the evidence of foundational identity is confirmed by a trained examiner.</t>
+    <t xml:space="preserve">The entity under assessment SHALL confirm the the evidence of foundational identity with the issuing authority AND SHALL validate the identity information against the authoritative record AND SHALL request the status of the Subject from the issuing authority.
+If confirmation with the issuing authority or validation of the identity information is not feasible, then the entity under assessment SHALL ensure that the evidence of foundational identity is confirmed by a trained examiner.</t>
   </si>
   <si>
     <t xml:space="preserve">IDRE</t>
@@ -2248,7 +2219,7 @@
     <t xml:space="preserve">IDRE.01</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST ensure that the identity information provided uniquely resolves to only one entity within its program/service population.</t>
+    <t xml:space="preserve">The entity under assessment SHALL ensure that the identity information provided uniquely resolves to only one entity within its program/service population.</t>
   </si>
   <si>
     <t xml:space="preserve">IDES</t>
@@ -2368,7 +2339,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST be a registered public sector  or private sector entity (e.g., a government department, agency, or ministry, a proprietorship, corporation, association, etc.).</t>
+    <t xml:space="preserve">The entity under assessment SHALL be a registered public sector  or private sector entity (e.g., a government department, agency, or ministry, a proprietorship, corporation, association, etc.).</t>
   </si>
   <si>
     <t xml:space="preserve">IDES.03</t>
@@ -2409,7 +2380,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST be a government department, agency, ministry, or other public sector entity operating under the authority of a Canadian federal, provincial, or territorial government, or a government-regulated private sector entity.</t>
+    <t xml:space="preserve">The entity under assessment SHALL be a government department, agency, ministry, or other public sector entity operating under the authority of a Canadian federal, provincial, or territorial government, or a government-regulated private sector entity.</t>
   </si>
   <si>
     <t xml:space="preserve">IDES.04</t>
@@ -2418,13 +2389,13 @@
     <t xml:space="preserve">PFID,OFID</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST be a provincial or territorial vital statistics registrar, IRCC, a provincial or territorial business registrar, or Corporations Canada.</t>
+    <t xml:space="preserve">The entity under assessment SHALL be a provincial or territorial vital statistics registrar, IRCC, a provincial or territorial business registrar, or Corporations Canada.</t>
   </si>
   <si>
     <t xml:space="preserve">IDES.05</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST ensure that the creation of the record of contextual identity is confirmed by and referenceable to a relevant event or activity.</t>
+    <t xml:space="preserve">The entity under assessment SHALL ensure that the creation of the record of contextual identity is confirmed by and referenceable to a relevant event or activity.</t>
   </si>
   <si>
     <t xml:space="preserve">IDES.06</t>
@@ -2433,7 +2404,7 @@
     <t xml:space="preserve">PFID</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST ensure that the creation of the record of foundational identity of a person is confirmed by and referenceable to one of the following events:
+    <t xml:space="preserve">The entity under assessment SHALL ensure that the creation of the record of foundational identity of a person is confirmed by and referenceable to one of the following events:
   ● Birth in Canada
   ● Acquired Status 
       o Canadian birth abroad (outside of Canada)
@@ -2442,7 +2413,7 @@
       o Citizenship
       o Permanent residency
       o Temporary residency (including protected persons)
-The entity under assessment MUST ensure that an inspection of all the relevant documents and evidence is conducted by a trained examiner using a risk-based approach.</t>
+The entity under assessment SHALL ensure that an inspection of all the relevant documents and evidence is conducted by a trained examiner using a risk-based approach.</t>
   </si>
   <si>
     <t xml:space="preserve">IDES.07</t>
@@ -2451,11 +2422,11 @@
     <t xml:space="preserve">OFID</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST ensure that the creation of the record of foundational identity of an organization is confirmed by and referenceable to one of the following events:
+    <t xml:space="preserve">The entity under assessment SHALL ensure that the creation of the record of foundational identity of an organization is confirmed by and referenceable to one of the following events:
   ● Incorporation
   ● Amalgamation (of one or more incoporated entities)
   ● Continuence (an incorporated entity moves from one Canadian jurisdiction to another jurisdiction)
-The entity under assessment MUST ensure that an inspection of all the relevant documents and evidence is conducted by a trained examiner using a risk-based approach.</t>
+The entity under assessment SHALL ensure that an inspection of all the relevant documents and evidence is conducted by a trained examiner using a risk-based approach.</t>
   </si>
   <si>
     <t xml:space="preserve">IDES.08</t>
@@ -2464,39 +2435,10 @@
     <t xml:space="preserve">IP1,IP2,IP3</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">The entity under assessment MUST ensure that the record of contextual identity</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">of a person contains the following minimum identity information:
+    <t xml:space="preserve">The entity under assessment SHALL ensure that the record of contextual identity of a person contains the following minimum identity information:
   ● PERSON NAME indicating the name by which a person is known or referred to
   ● The initiating party for the establishment of the identity record
   ● Any other Identity information requirements that are specified in applicable regulations</t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">IDES.09</t>
@@ -2505,7 +2447,7 @@
     <t xml:space="preserve">IO1,IO2,IO3</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST ensure that the record of contextual identity of an organization contains the following minimum identity information:
+    <t xml:space="preserve">The entity under assessment SHALL ensure that the record of contextual identity of an organization contains the following minimum identity information:
   ● LEGAL NAME indicating the name by which an organization is legally recognized or referred to
   ● JURISDICTION OF INCORPORATION indicating the jurisdiction in which the organization is incorporated
   ● The initiating party for the establishment of the identity record
@@ -2518,7 +2460,7 @@
     <t xml:space="preserve">PFID  </t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST ensure that the record of foundational identity of a person contains the following minimum identity information:
+    <t xml:space="preserve">The entity under assessment SHALL ensure that the record of foundational identity of a person contains the following minimum identity information:
 For Birth in Canada: 
   ● ASSIGNED IDENTIFIER that uniquely distinguishes a person from all other persons within a population
   ● PERSON NAME indicating the name by which a person is registered
@@ -2560,35 +2502,7 @@
     <t xml:space="preserve">IDES.11</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">The entity under assessment MUST ensure that the record of foundational identity of an organization</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">contains the following minimum identity information:
+    <t xml:space="preserve">The entity under assessment SHALL ensure that the record of foundational identity of an organization contains the following minimum identity information:
   ● ASSIGNED IDENTIFIER that uniquely distinguishes an organization from all other organizations within a population
   ● LEGAL NAME indicating the name by which an organization is legally recognized or referred to
   ● JURISDICTION OF INCORPORATION indicating the jurisdiction in which the organization is incorporated 
@@ -2600,7 +2514,6 @@
   ● ORGANIZATION TYPE (e.g., Association, Corporation, Trust, Sole Proprietorships, Partnerships, Co-Operatives, Credit Unions, Other, etc.)
   ● The initiating party for the establishment of the identity record
   ● Any other Identity information requirements that are specified in applicable regulations</t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">IDVE</t>
@@ -2660,12 +2573,12 @@
     <t xml:space="preserve">IDVE.03</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST use at least one of the following methods to confirm that the identity information of a person is under the control of the Subject: 
+    <t xml:space="preserve">The entity under assessment SHALL use at least one of the following methods to confirm that the identity information of a person is under the control of the Subject: 
  ● Knowledge-based confirmation
  ● Biological or behavioural characteristic confirmation
  ● Physical possession confirmation
  ● Trusted referee confirmation
-If the above methods are not feasible then the entity under assessment MUST define and document alternative methods in an exception process. These alternative methods MAY include:
+If the above methods are not feasible then the entity under assessment SHALL define and document alternative methods in an exception process. These alternative methods MAY include:
  ● Additional safeguards
  ● Compensating factors</t>
   </si>
@@ -2711,7 +2624,7 @@
     <t xml:space="preserve">IDMA.01</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST ensure that records of identity are updated in a timely manner.</t>
+    <t xml:space="preserve">The entity under assessment SHALL ensure that records of identity are updated in a timely manner.</t>
   </si>
   <si>
     <t xml:space="preserve">IDMA.02</t>
@@ -2743,7 +2656,7 @@
     <t xml:space="preserve">IP2,IP3</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST confirm with the foundational identity authority any changes to the identity information of a person for the following events:
+    <t xml:space="preserve">The entity under assessment SHALL confirm with the foundational identity authority any changes to the identity information of a person for the following events:
   ● Name change 
   ● Gender change
   ● Death</t>
@@ -2755,7 +2668,7 @@
     <t xml:space="preserve">IO2,IO3</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST confirm with the foundational identity authority any changes to the identity information of an organization for the following events:
+    <t xml:space="preserve">The entity under assessment SHALL confirm with the foundational identity authority any changes to the identity information of an organization for the following events:
   ● Legal Name change 
   ● Registered Office Address change
   ● Board of Directors Composition change
@@ -2773,19 +2686,19 @@
     <t xml:space="preserve">IDMA.07</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST ensure that the identity information is periodically updated from the authoritative record of identity.</t>
+    <t xml:space="preserve">The entity under assessment SHALL ensure that the identity information is periodically updated from the authoritative record of identity.</t>
   </si>
   <si>
     <t xml:space="preserve">IDMA.08</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST ensure that they undertake a reassessment of the updated identity information and, where warranted, they MUST ensure that appropriate administrative action is subsequently taken.</t>
+    <t xml:space="preserve">The entity under assessment SHALL ensure that they undertake a reassessment of the updated identity information and, where warranted, they SHALL ensure that appropriate administrative action is subsequently taken.</t>
   </si>
   <si>
     <t xml:space="preserve">IDMA.09</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST record the initiating party of the identity record modification and the date of the modification of the identity record.</t>
+    <t xml:space="preserve">The entity under assessment SHALL record the initiating party of the identity record modification and the date of the modification of the identity record.</t>
   </si>
   <si>
     <t xml:space="preserve">IDLI</t>
@@ -2828,31 +2741,31 @@
     <t xml:space="preserve">IDLI.01</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST ensure that the identity information of the identity records being linked is substantialy equivalent. </t>
+    <t xml:space="preserve">The entity under assessment SHALL ensure that the identity information of the identity records being linked is substantialy equivalent. </t>
   </si>
   <si>
     <t xml:space="preserve">IDLI.02</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment SHOULD perform identity verification to ensure that the assigned identitfiers are referencing the same entity prior to linking. Identity verification MUST meet or exceed the identity verification requirements applicable to the IP1 (for persons) qualifier in Identity Verification. </t>
+    <t xml:space="preserve">The entity under assessment SHOULD perform identity verification to ensure that the assigned identitfiers are referencing the same entity prior to linking. Identity verification SHALL meet or exceed the identity verification requirements applicable to the IP1 (for persons) qualifier in Identity Verification. </t>
   </si>
   <si>
     <t xml:space="preserve">IDLI.03</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST perform identity verification to ensure that the assigned identitfiers are referencing the same entity prior to linking. Identity verification MUST meet or exceed the identity verification requirements applicable to the IP2 (for persons) qualifier in Identity Verification. </t>
+    <t xml:space="preserve">The entity under assessment SHALL perform identity verification to ensure that the assigned identitfiers are referencing the same entity prior to linking. Identity verification SHALL meet or exceed the identity verification requirements applicable to the IP2 (for persons) qualifier in Identity Verification. </t>
   </si>
   <si>
     <t xml:space="preserve">IDLI.04</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST perform identity verification to ensure that the assigned identitfiers are referencing the same entity prior to linking. Identity verification MUST meet or exceed the identity verification requirements applicable to the IP3 (for persons) qualifier in Identity Verification. </t>
+    <t xml:space="preserve">The entity under assessment SHALL perform identity verification to ensure that the assigned identitfiers are referencing the same entity prior to linking. Identity verification SHALL meet or exceed the identity verification requirements applicable to the IP3 (for persons) qualifier in Identity Verification. </t>
   </si>
   <si>
     <t xml:space="preserve">IDLI.05</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST use confirmation methods that are independent of each other (the use of one method cannot compromise the use of another).</t>
+    <t xml:space="preserve">The entity under assessment SHALL use confirmation methods that are independent of each other (the use of one method cannot compromise the use of another).</t>
   </si>
   <si>
     <t xml:space="preserve">REDG</t>
@@ -2883,19 +2796,19 @@
     <t xml:space="preserve">R2,R3</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST adhere to applicable relationship management controls, standards, and guidelines, and MUST have an auditable process to demonstrate adherence.</t>
+    <t xml:space="preserve">The entity under assessment SHALL adhere to applicable relationship management controls, standards, and guidelines, and SHALL have an auditable process to demonstrate adherence.</t>
   </si>
   <si>
     <t xml:space="preserve">REDG.03</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST provide a list of the applicable relationship management controls, standards, and guidelines that are in effect.</t>
+    <t xml:space="preserve">The entity under assessment SHALL provide a list of the applicable relationship management controls, standards, and guidelines that are in effect.</t>
   </si>
   <si>
     <t xml:space="preserve">REDG.04</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST demonstrate the equivalency of the applicable relationship management controls, standards, and guidelines to those used by the assessor.</t>
+    <t xml:space="preserve">The entity under assessment SHALL demonstrate the equivalency of the applicable relationship management controls, standards, and guidelines to those used by the assessor.</t>
   </si>
   <si>
     <t xml:space="preserve">REDG.05</t>
@@ -2922,7 +2835,7 @@
     <t xml:space="preserve">R1,R2,R3</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST have procedures in place to ensure that service provision is granted or denied, based on relationship status (i.e., valid, suspended, reinstated, or revoked).</t>
+    <t xml:space="preserve">The entity under assessment SHALL have procedures in place to ensure that service provision is granted or denied, based on relationship status (i.e., valid, suspended, reinstated, or revoked).</t>
   </si>
   <si>
     <t xml:space="preserve">REID</t>
@@ -2966,7 +2879,7 @@
     <t xml:space="preserve">REID.01</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST specify the relationship context of the program or service, specifically, the relationships of interest and their definitions within the context of the program or service. </t>
+    <t xml:space="preserve">The entity under assessment SHALL specify the relationship context of the program or service, specifically, the relationships of interest and their definitions within the context of the program or service. </t>
   </si>
   <si>
     <t xml:space="preserve">REID.02</t>
@@ -2976,13 +2889,13 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST specify the program or service identity context of the entities involved in the relationships (see Identity Information Determination).</t>
+    <t xml:space="preserve">The entity under assessment SHALL specify the program or service identity context of the entities involved in the relationships (see Identity Information Determination).</t>
   </si>
   <si>
     <t xml:space="preserve">REID.03</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST define the identity information requirements of the entities involved in the relationships (i.e., the set of identity attributes) (see Identity Information Determination).  </t>
+    <t xml:space="preserve">The entity under assessment SHALL define the identity information requirements of the entities involved in the relationships (i.e., the set of identity attributes) (see Identity Information Determination).  </t>
   </si>
   <si>
     <t xml:space="preserve">REID.04</t>
@@ -2991,13 +2904,13 @@
     <t xml:space="preserve">R1,R2,R3 </t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST define the relationship information requirements (i.e., the set of relationship attributes) of the program or service. </t>
+    <t xml:space="preserve">The entity under assessment SHALL define the relationship information requirements (i.e., the set of relationship attributes) of the program or service. </t>
   </si>
   <si>
     <t xml:space="preserve">REID.05</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST define the set of identity attributes and relationship attributes that will be used to uniquely distinguish a particular relationship instance within the program/service  relationship context. This set of identity attributes and relationship attributes is referred to as the relationship identifier.</t>
+    <t xml:space="preserve">The entity under assessment SHALL define the set of identity attributes and relationship attributes that will be used to uniquely distinguish a particular relationship instance within the program/service  relationship context. This set of identity attributes and relationship attributes is referred to as the relationship identifier.</t>
   </si>
   <si>
     <t xml:space="preserve">REED</t>
@@ -3061,25 +2974,25 @@
     <t xml:space="preserve">REED.01</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST determine the acceptable evidence of the relationship (whether physical or electronic) for its programs and services.</t>
+    <t xml:space="preserve">The entity under assessment SHALL determine the acceptable evidence of the relationship (whether physical or electronic) for its programs and services.</t>
   </si>
   <si>
     <t xml:space="preserve">REED.02</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST identify the acceptable information providers from which an assertion of the existence/ suspension/ reinstatement/ revocation of the relationship, within the context of the program/service, will be accepted.</t>
+    <t xml:space="preserve">The entity under assessment SHALL identify the acceptable information providers from which an assertion of the existence/ suspension/ reinstatement/ revocation of the relationship, within the context of the program/service, will be accepted.</t>
   </si>
   <si>
     <t xml:space="preserve">REED.03</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST identify the acceptable information providers from which identity attributes required by the relationship domain processes will be accepted.</t>
+    <t xml:space="preserve">The entity under assessment SHALL identify the acceptable information providers from which identity attributes required by the relationship domain processes will be accepted.</t>
   </si>
   <si>
     <t xml:space="preserve">REED.04</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST identify the acceptable information providers from which relationship attributes required to by the relationship domain processes will be accepted.</t>
+    <t xml:space="preserve">The entity under assessment SHALL identify the acceptable information providers from which relationship attributes required to by the relationship domain processes will be accepted.</t>
   </si>
   <si>
     <t xml:space="preserve">REEA</t>
@@ -3146,37 +3059,37 @@
     <t xml:space="preserve">REEA.01</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST ensure that the entities presenting evidence are acceptable information providers as defined in Relationship Evidence Determination.  </t>
+    <t xml:space="preserve">The entity under assessment SHALL ensure that the entities presenting evidence are acceptable information providers as defined in Relationship Evidence Determination.  </t>
   </si>
   <si>
     <t xml:space="preserve">REEA.02</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST confirm that the evidence of the relationship conforms to the evidence defined in Relationship Evidence Determination</t>
+    <t xml:space="preserve">The entity under assessment SHALL confirm that the evidence of the relationship conforms to the evidence defined in Relationship Evidence Determination</t>
   </si>
   <si>
     <t xml:space="preserve">REEA.03</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST NOT restrict what is provided as evidence of the relationship.</t>
+    <t xml:space="preserve">The entity under assessment SHALL NOT restrict what is provided as evidence of the relationship.</t>
   </si>
   <si>
     <t xml:space="preserve">REEA.04</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST ensure that the identity evidence presented meets or exceeds the requirements applicable to the IP1 (for persons) or IO1 (for organizations) qualifier(s) in Identity Evidence Acceptance.</t>
+    <t xml:space="preserve">The entity under assessment SHALL ensure that the identity evidence presented meets or exceeds the requirements applicable to the IP1 (for persons) or IO1 (for organizations) qualifier(s) in Identity Evidence Acceptance.</t>
   </si>
   <si>
     <t xml:space="preserve">REEA.05</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST ensure that the identity evidence presented meets or exceeds the requirements applicable to the IP2 (for persons) or IO2 (for organizations) qualifier(s) in Identity Evidence Acceptance.</t>
+    <t xml:space="preserve">The entity under assessment SHALL ensure that the identity evidence presented meets or exceeds the requirements applicable to the IP2 (for persons) or IO2 (for organizations) qualifier(s) in Identity Evidence Acceptance.</t>
   </si>
   <si>
     <t xml:space="preserve">REEA.06</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST ensure that the identity evidence presented meets the requirements applicable to the IP3 (for persons) or IO3 (for organizations) qualifier(s) in Identity Evidence Acceptance.</t>
+    <t xml:space="preserve">The entity under assessment SHALL ensure that the identity evidence presented meets the requirements applicable to the IP3 (for persons) or IO3 (for organizations) qualifier(s) in Identity Evidence Acceptance.</t>
   </si>
   <si>
     <t xml:space="preserve">REIV</t>
@@ -3243,25 +3156,25 @@
     <t xml:space="preserve">REIV.01</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST ensure that the identity information provided meets or exceeds the requirements applicable to the IP1 (for persons) or IO1 (for organizations) qualifier(s) in Identity Information Validation.</t>
+    <t xml:space="preserve">The entity under assessment SHALL ensure that the identity information provided meets or exceeds the requirements applicable to the IP1 (for persons) or IO1 (for organizations) qualifier(s) in Identity Information Validation.</t>
   </si>
   <si>
     <t xml:space="preserve">REIV.02</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST ensure that the identity information provided meets or exceeds the requirements applicable to the IP2 (for persons) or IO2 (for organizations) qualifier(s) in Identity Information Validation.</t>
+    <t xml:space="preserve">The entity under assessment SHALL ensure that the identity information provided meets or exceeds the requirements applicable to the IP2 (for persons) or IO2 (for organizations) qualifier(s) in Identity Information Validation.</t>
   </si>
   <si>
     <t xml:space="preserve">REIV.03</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST ensure that the identity information provided meets the requirements applicable to the IP3 (for persons) or IO3 (for organizations) qualifier(s) in Identity Information Validation.</t>
+    <t xml:space="preserve">The entity under assessment SHALL ensure that the identity information provided meets the requirements applicable to the IP3 (for persons) or IO3 (for organizations) qualifier(s) in Identity Information Validation.</t>
   </si>
   <si>
     <t xml:space="preserve">REIV.04</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST confirm that the assertions of relationship type and status acceptably match all instances of relationship evidence provided.</t>
+    <t xml:space="preserve">The entity under assessment SHALL confirm that the assertions of relationship type and status acceptably match all instances of relationship evidence provided.</t>
   </si>
   <si>
     <t xml:space="preserve">REIV.05</t>
@@ -3333,7 +3246,7 @@
     <t xml:space="preserve">RERE.01</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST ensure that the relationship information and identity information provided uniquely resolves to only one relationship instance within its program/service population.</t>
+    <t xml:space="preserve">The entity under assessment SHALL ensure that the relationship information and identity information provided uniquely resolves to only one relationship instance within its program/service population.</t>
   </si>
   <si>
     <t xml:space="preserve">REES</t>
@@ -3415,25 +3328,25 @@
     <t xml:space="preserve">REES.05</t>
   </si>
   <si>
-    <t xml:space="preserve">When establishing the record of identity for the purposes of relationship establishment, the entity under assessment MUST meet or exceed the requirements applicable to the IP1 (for persons) or IO1 (for organizations) qualifier(s) in Identity Establishment.</t>
+    <t xml:space="preserve">When establishing the record of identity for the purposes of relationship establishment, the entity under assessment SHALL meet or exceed the requirements applicable to the IP1 (for persons) or IO1 (for organizations) qualifier(s) in Identity Establishment.</t>
   </si>
   <si>
     <t xml:space="preserve">REES.06</t>
   </si>
   <si>
-    <t xml:space="preserve">When establishing the record of identity for the purposes of relationship establishment, the entity under assessment MUST meet or exceed the requirements applicable to the IP2 (for persons) or IO2 (for organizations) qualifier(s) in Identity Establishment.</t>
+    <t xml:space="preserve">When establishing the record of identity for the purposes of relationship establishment, the entity under assessment SHALL meet or exceed the requirements applicable to the IP2 (for persons) or IO2 (for organizations) qualifier(s) in Identity Establishment.</t>
   </si>
   <si>
     <t xml:space="preserve">REES.07</t>
   </si>
   <si>
-    <t xml:space="preserve">When establishing the record of identity for the purposes of relationship establishment, the entity under assessment MUST meet or exceed the requirements applicable to the IP3 (for persons) or IO3 (for organizations) qualifier(s) in Identity Establishment.</t>
+    <t xml:space="preserve">When establishing the record of identity for the purposes of relationship establishment, the entity under assessment SHALL meet or exceed the requirements applicable to the IP3 (for persons) or IO3 (for organizations) qualifier(s) in Identity Establishment.</t>
   </si>
   <si>
     <t xml:space="preserve">REES.08</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST ensure that the record of the relationship includes, at a minimum:
+    <t xml:space="preserve">The entity under assessment SHALL ensure that the record of the relationship includes, at a minimum:
   ● names of the entities in the relationship
   ● type of relationship, based on the defined relationship context of the program or service
   ● identity or relationship identifiers appropriate to program or service context
@@ -3506,19 +3419,19 @@
     <t xml:space="preserve">REVE.01</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST ensure that the identity verification of Subjects who are persons, meets or exceeds the requirements applicable to the IP1 (for persons) qualifier in Identity Verification.</t>
+    <t xml:space="preserve">The entity under assessment SHALL ensure that the identity verification of Subjects who are persons, meets or exceeds the requirements applicable to the IP1 (for persons) qualifier in Identity Verification.</t>
   </si>
   <si>
     <t xml:space="preserve">REVE.02</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST ensure that the identity verification of Subjects who are persons, meets or exceeds the requirements applicable to the IP2 (for persons) qualifier in Identity Verification.</t>
+    <t xml:space="preserve">The entity under assessment SHALL ensure that the identity verification of Subjects who are persons, meets or exceeds the requirements applicable to the IP2 (for persons) qualifier in Identity Verification.</t>
   </si>
   <si>
     <t xml:space="preserve">REVE.03</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST ensure that the identity verification of Subjects who are persons, meets the requirements applicable to the IP3 (for persons) qualifier in Identity Verification.</t>
+    <t xml:space="preserve">The entity under assessment SHALL ensure that the identity verification of Subjects who are persons, meets the requirements applicable to the IP3 (for persons) qualifier in Identity Verification.</t>
   </si>
   <si>
     <t xml:space="preserve">RECO</t>
@@ -3628,7 +3541,7 @@
     <t xml:space="preserve">REMA.01</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST ensure that records of relationship are updated in a timely manner.</t>
+    <t xml:space="preserve">The entity under assessment SHALL ensure that records of relationship are updated in a timely manner.</t>
   </si>
   <si>
     <t xml:space="preserve">REMA.02</t>
@@ -3640,25 +3553,25 @@
     <t xml:space="preserve">REMA.03</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST ensure that the procedure for the maintenance of identity information, meets or exceeds the requirements applicable to the IP1 (for persons) or IO1 (for organizations) qualifier(s) in Identity Maintenance.</t>
+    <t xml:space="preserve">The entity under assessment SHALL ensure that the procedure for the maintenance of identity information, meets or exceeds the requirements applicable to the IP1 (for persons) or IO1 (for organizations) qualifier(s) in Identity Maintenance.</t>
   </si>
   <si>
     <t xml:space="preserve">REMA.04</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST ensure that the procedure for the maintenance of identity information, meets or exceeds the requirements applicable to the IP2 (for persons) or IO2 (for organizations) qualifier(s) in Identity Maintenance.</t>
+    <t xml:space="preserve">The entity under assessment SHALL ensure that the procedure for the maintenance of identity information, meets or exceeds the requirements applicable to the IP2 (for persons) or IO2 (for organizations) qualifier(s) in Identity Maintenance.</t>
   </si>
   <si>
     <t xml:space="preserve">REMA.05</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST ensure that the procedure for the maintenance of identity information, meets the requirements applicable to the IP3 (for persons) or IO3 (for organizations) qualifier(s) in Identity Maintenance.</t>
+    <t xml:space="preserve">The entity under assessment SHALL ensure that the procedure for the maintenance of identity information, meets the requirements applicable to the IP3 (for persons) or IO3 (for organizations) qualifier(s) in Identity Maintenance.</t>
   </si>
   <si>
     <t xml:space="preserve">REMA.06</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST record the initiating party for the relationship record modification, and the date of modification of the relationship record.</t>
+    <t xml:space="preserve">The entity under assessment SHALL record the initiating party for the relationship record modification, and the date of modification of the relationship record.</t>
   </si>
   <si>
     <t xml:space="preserve">RESU</t>
@@ -3676,13 +3589,13 @@
     <t xml:space="preserve">RESU.01</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST have the ability to suspend the relationship (for example, due to the expiry date having been exceeded or the detection of suspicious activity).</t>
+    <t xml:space="preserve">The entity under assessment SHALL have the ability to suspend the relationship (for example, due to the expiry date having been exceeded or the detection of suspicious activity).</t>
   </si>
   <si>
     <t xml:space="preserve">RESU.02</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST suspend the relationship if the entity under assessment detects indications of compromised information or compromised automated processing components.</t>
+    <t xml:space="preserve">The entity under assessment SHALL suspend the relationship if the entity under assessment detects indications of compromised information or compromised automated processing components.</t>
   </si>
   <si>
     <t xml:space="preserve">RESU.03</t>
@@ -3694,7 +3607,7 @@
     <t xml:space="preserve">RESU.04</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST perform Identity Verification of the party in the relationship making the relationship suspension request.</t>
+    <t xml:space="preserve">The entity under assessment SHALL perform Identity Verification of the party in the relationship making the relationship suspension request.</t>
   </si>
   <si>
     <t xml:space="preserve">RESU.05</t>
@@ -3706,7 +3619,7 @@
     <t xml:space="preserve">RESU.06</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST undertake a reassessment of the relationship, potentially leading to suspension, when evidence of a potential change to to the identity attributes or relationship attributes is made known from an acceptable information provider.</t>
+    <t xml:space="preserve">The entity under assessment SHALL undertake a reassessment of the relationship, potentially leading to suspension, when evidence of a potential change to to the identity attributes or relationship attributes is made known from an acceptable information provider.</t>
   </si>
   <si>
     <t xml:space="preserve">RESU.07</t>
@@ -3736,7 +3649,7 @@
     <t xml:space="preserve">RESU.11</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST ensure that the suspended relationship undergoes a timely reassessment, based on the entity under assessment's formal policy and procedures, leading to either relationship reinstatement or relationship revocation.</t>
+    <t xml:space="preserve">The entity under assessment SHALL ensure that the suspended relationship undergoes a timely reassessment, based on the entity under assessment's formal policy and procedures, leading to either relationship reinstatement or relationship revocation.</t>
   </si>
   <si>
     <t xml:space="preserve">RERI</t>
@@ -3805,7 +3718,7 @@
     <t xml:space="preserve">RERI.01</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST have the ability to reinstate the suspended relationship.</t>
+    <t xml:space="preserve">The entity under assessment SHALL have the ability to reinstate the suspended relationship.</t>
   </si>
   <si>
     <t xml:space="preserve">RERI.02</t>
@@ -3817,19 +3730,19 @@
     <t xml:space="preserve">RERI.03</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST perform Identity Verification of the party in the relationship making the relationship reinstatement request.</t>
+    <t xml:space="preserve">The entity under assessment SHALL perform Identity Verification of the party in the relationship making the relationship reinstatement request.</t>
   </si>
   <si>
     <t xml:space="preserve">RERI.04</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST ensure that the reinstatement of the relationship can only occur after reassessment based on the current evidence and the execution of the requirements in Relationship Evidence Acceptance and Relationship Information Validation.</t>
+    <t xml:space="preserve">The entity under assessment SHALL ensure that the reinstatement of the relationship can only occur after reassessment based on the current evidence and the execution of the requirements in Relationship Evidence Acceptance and Relationship Information Validation.</t>
   </si>
   <si>
     <t xml:space="preserve">RERI.05</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST ensure that relationship reinstatement only applies to those relationships that are in a suspended state (i.e., revoked relationships cannot be reinstated, they must be recreated).</t>
+    <t xml:space="preserve">The entity under assessment SHALL ensure that relationship reinstatement only applies to those relationships that are in a suspended state (i.e., revoked relationships cannot be reinstated, they SHALL be recreated).</t>
   </si>
   <si>
     <t xml:space="preserve">RERI.06</t>
@@ -3887,7 +3800,7 @@
     <t xml:space="preserve">RERV.01</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST have the ability to revoke the relationship (for example, due to the expiry date having been exceeded or the detection of suspicious activity).</t>
+    <t xml:space="preserve">The entity under assessment SHALL have the ability to revoke the relationship (for example, due to the expiry date having been exceeded or the detection of suspicious activity).</t>
   </si>
   <si>
     <t xml:space="preserve">RERV.02</t>
@@ -3905,13 +3818,13 @@
     <t xml:space="preserve">RERV.04</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST perform Identity Verification of the party in the relationship making the relationship revocation request.</t>
+    <t xml:space="preserve">The entity under assessment SHALL perform Identity Verification of the party in the relationship making the relationship revocation request.</t>
   </si>
   <si>
     <t xml:space="preserve">RERV.05</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST ensure that relationship revocation can only occur based on relevant policy, law, or regulation.</t>
+    <t xml:space="preserve">The entity under assessment SHALL ensure that relationship revocation can only occur based on relevant policy, law, or regulation.</t>
   </si>
   <si>
     <t xml:space="preserve">RERV.06</t>
@@ -3929,7 +3842,7 @@
     <t xml:space="preserve">RERV.08</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST inform the parties in the relationship of the change in the relationship status.</t>
+    <t xml:space="preserve">The entity under assessment SHALL inform the parties in the relationship of the change in the relationship status.</t>
   </si>
   <si>
     <t xml:space="preserve">RERV.09</t>
@@ -3962,19 +3875,19 @@
     <t xml:space="preserve">C2,C3</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST adhere to applicable credential management controls, standards, and guidelines, and MUST have an auditable process to demonstrate adherence.</t>
+    <t xml:space="preserve">The entity under assessment SHALL adhere to applicable credential management controls, standards, and guidelines, and SHALL have an auditable process to demonstrate adherence.</t>
   </si>
   <si>
     <t xml:space="preserve">CRDG.03</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST provide a list of the applicable credential management controls, standards, and guidelines that are in effect.</t>
+    <t xml:space="preserve">The entity under assessment SHALL provide a list of the applicable credential management controls, standards, and guidelines that are in effect.</t>
   </si>
   <si>
     <t xml:space="preserve">CRDG.04</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST demonstrate the equivalency of the applicable credential management controls, standards, and guidelines to those used by the assessor. </t>
+    <t xml:space="preserve">The entity under assessment SHALL demonstrate the equivalency of the applicable credential management controls, standards, and guidelines to those used by the assessor. </t>
   </si>
   <si>
     <t xml:space="preserve">CRDG.05</t>
@@ -3986,7 +3899,7 @@
     <t xml:space="preserve">CRDG.06</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST monitor for indications of credential misuse or compromise.</t>
+    <t xml:space="preserve">The entity under assessment SHALL monitor for indications of credential misuse or compromise.</t>
   </si>
   <si>
     <t xml:space="preserve">CRDG.07</t>
@@ -4007,7 +3920,7 @@
     <t xml:space="preserve">CRDG.09</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST log and retain for a predefined period of time all credential events. </t>
+    <t xml:space="preserve">The entity under assessment SHALL log and retain for a predefined period of time all credential events. </t>
   </si>
   <si>
     <t xml:space="preserve">CRIS</t>
@@ -4046,19 +3959,19 @@
     <t xml:space="preserve">CRIS.01</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST ensure that the credential is referenceable to a relevant event or activity.</t>
+    <t xml:space="preserve">The entity under assessment SHALL ensure that the credential is referenceable to a relevant event or activity.</t>
   </si>
   <si>
     <t xml:space="preserve">CRIS.02</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST ensure that the credential identifies the Issuer. </t>
+    <t xml:space="preserve">The entity under assessment SHALL ensure that the credential identifies the Issuer. </t>
   </si>
   <si>
     <t xml:space="preserve">CRIS.03</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST ensure that the credential has a defined validity period.</t>
+    <t xml:space="preserve">The entity under assessment SHALL ensure that the credential has a defined validity period.</t>
   </si>
   <si>
     <t xml:space="preserve">CRIS.04</t>
@@ -4070,19 +3983,19 @@
     <t xml:space="preserve">CRIS.05</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST ensure that the credential is tamper-evident.</t>
+    <t xml:space="preserve">The entity under assessment SHALL ensure that the credential is tamper-evident.</t>
   </si>
   <si>
     <t xml:space="preserve">CRIS.06</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST ensure that the credential is unique within a specified population.</t>
+    <t xml:space="preserve">The entity under assessment SHALL ensure that the credential is unique within a specified population.</t>
   </si>
   <si>
     <t xml:space="preserve">CRIS.07</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST ensure that the credential is provided to the rightful Holder.</t>
+    <t xml:space="preserve">The entity under assessment SHALL ensure that the credential is provided to the rightful Holder.</t>
   </si>
   <si>
     <t xml:space="preserve">CRAB</t>
@@ -4151,13 +4064,13 @@
     <t xml:space="preserve">CRAB.01</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST ensure that at least one authenticator is bound to the credential.</t>
+    <t xml:space="preserve">The entity under assessment SHALL ensure that at least one authenticator is bound to the credential.</t>
   </si>
   <si>
     <t xml:space="preserve">CRAB.02</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MAY provide to the Holder the ability to update the authenticators bound to the credential. In this case, the Credential Validation and Credential Verfication processes MUST be performed first.</t>
+    <t xml:space="preserve">The entity under assessment MAY provide to the Holder the ability to update the authenticators bound to the credential. In this case, the Credential Validation and Credential Verfication processes SHALL be performed first.</t>
   </si>
   <si>
     <t xml:space="preserve">CRAB.03</t>
@@ -4169,13 +4082,13 @@
     <t xml:space="preserve">CRAB.04</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment SHOULD require the Holder to complete any administrator-initiated credential authenticator binding (e.g., the Holder must supply a new password when the administrator initiates a password reset).</t>
+    <t xml:space="preserve">The entity under assessment SHOULD require the Holder to complete any administrator-initiated credential authenticator binding (e.g., the Holder SHALL supply a new password when the administrator initiates a password reset).</t>
   </si>
   <si>
     <t xml:space="preserve">CRAB.05</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST require the Holder to complete any administrator-initiated credential authenticator binding (e.g., the Holder must supply a new password when the administrator initiates a password reset).</t>
+    <t xml:space="preserve">The entity under assessment SHALL require the Holder to complete any administrator-initiated credential authenticator binding (e.g., the Holder SHALL supply a new password when the administrator initiates a password reset).</t>
   </si>
   <si>
     <t xml:space="preserve">CRVA</t>
@@ -4195,13 +4108,13 @@
     <t xml:space="preserve">CRVA.01</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST ensure, using acceptable methods, that the credential is not tampered with, corrupted, or modified. Examples of acceptable methods are cryptographic methods or examination by a trained examiner.</t>
+    <t xml:space="preserve">The entity under assessment SHALL ensure, using acceptable methods, that the credential is not tampered with, corrupted, or modified. Examples of acceptable methods are cryptographic methods or examination by a trained examiner.</t>
   </si>
   <si>
     <t xml:space="preserve">CRVA.02</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST be able to determine if the credential is suspended or revoked.</t>
+    <t xml:space="preserve">The entity under assessment SHALL be able to determine if the credential is suspended or revoked.</t>
   </si>
   <si>
     <t xml:space="preserve">CRVE</t>
@@ -4246,19 +4159,19 @@
     <t xml:space="preserve">CRVE.01</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST ensure that the Holder has demonstrated control over the credential by means of one or more authenticators.</t>
+    <t xml:space="preserve">The entity under assessment SHALL ensure that the Holder has demonstrated control over the credential by means of one or more authenticators.</t>
   </si>
   <si>
     <t xml:space="preserve">CRVE.02</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST inform the Holder when the Holder has demostrated control over the credential by means of one or more authenticators.</t>
+    <t xml:space="preserve">The entity under assessment SHALL inform the Holder when the Holder has demostrated control over the credential by means of one or more authenticators.</t>
   </si>
   <si>
     <t xml:space="preserve">CRVE.03</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST indicate an authentication failure when the credential is suspended or revoked, or when credential misuse or compromise is detected.</t>
+    <t xml:space="preserve">The entity under assessment SHALL indicate an authentication failure when the credential is suspended or revoked, or when credential misuse or compromise is detected.</t>
   </si>
   <si>
     <t xml:space="preserve">CRMA</t>
@@ -4276,7 +4189,7 @@
     <t xml:space="preserve">CRMA.01</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST ensure that the credential attributes of the credential are updated in a timely manner.</t>
+    <t xml:space="preserve">The entity under assessment SHALL ensure that the credential attributes of the credential are updated in a timely manner.</t>
   </si>
   <si>
     <t xml:space="preserve">CRMA.02</t>
@@ -4288,7 +4201,7 @@
     <t xml:space="preserve">CRMA.03</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST record the initiating party of the credential attribute modification, and the date of modification.</t>
+    <t xml:space="preserve">The entity under assessment SHALL record the initiating party of the credential attribute modification, and the date of modification.</t>
   </si>
   <si>
     <t xml:space="preserve">CRSU</t>
@@ -4334,13 +4247,13 @@
     <t xml:space="preserve">CRSU.01</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST have the ability to suspend the credential (for example, due to the expiry date having been exceeded or the detection of suspicious activity).</t>
+    <t xml:space="preserve">The entity under assessment SHALL have the ability to suspend the credential (for example, due to the expiry date having been exceeded or the detection of suspicious activity).</t>
   </si>
   <si>
     <t xml:space="preserve">CRSU.02</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST suspend the credential if the entity under assessment detects indications of compromised information or compromised automated processing components.</t>
+    <t xml:space="preserve">The entity under assessment SHALL suspend the credential if the entity under assessment detects indications of compromised information or compromised automated processing components.</t>
   </si>
   <si>
     <t xml:space="preserve">CRSU.03</t>
@@ -4352,7 +4265,7 @@
     <t xml:space="preserve">CRSU.04</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST perform Identity Verification of the Holder making the credential suspension request.</t>
+    <t xml:space="preserve">The entity under assessment SHALL perform Identity Verification of the Holder making the credential suspension request.</t>
   </si>
   <si>
     <t xml:space="preserve">CRSU.05</t>
@@ -4364,7 +4277,7 @@
     <t xml:space="preserve">CRSU.06</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST undertake a reassessment of the credential, potentially leading to suspension, when evidence of a potential change to the identity attributes or credential attributes is made known from an acceptable information provider.</t>
+    <t xml:space="preserve">The entity under assessment SHALL undertake a reassessment of the credential, potentially leading to suspension, when evidence of a potential change to the identity attributes or credential attributes is made known from an acceptable information provider.</t>
   </si>
   <si>
     <t xml:space="preserve">CRSU.07</t>
@@ -4388,7 +4301,7 @@
     <t xml:space="preserve">CRSU.10</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST ensure that the suspended credential undergoes a timely reassessment, based on the entity under assessment's formal policy and procedures, leading to either credential recovery or credential revocation.</t>
+    <t xml:space="preserve">The entity under assessment SHALL ensure that the suspended credential undergoes a timely reassessment, based on the entity under assessment's formal policy and procedures, leading to either credential recovery or credential revocation.</t>
   </si>
   <si>
     <t xml:space="preserve">CRRC</t>
@@ -4458,7 +4371,7 @@
     <t xml:space="preserve">CRRC.01</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST have the ability to recover the suspended credential.</t>
+    <t xml:space="preserve">The entity under assessment SHALL have the ability to recover the suspended credential.</t>
   </si>
   <si>
     <t xml:space="preserve">CRRC.02</t>
@@ -4470,19 +4383,19 @@
     <t xml:space="preserve">CRRC.03</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST perform Identity Verification of the Holder making the credential recovery request.</t>
+    <t xml:space="preserve">The entity under assessment SHALL perform Identity Verification of the Holder making the credential recovery request.</t>
   </si>
   <si>
     <t xml:space="preserve">CRRC.04</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST ensure that recovery of the credential can only occur after reassessment based on the current evidence and the execution of the requirements in Credential Validation.</t>
+    <t xml:space="preserve">The entity under assessment SHALL ensure that recovery of the credential can only occur after reassessment based on the current evidence and the execution of the requirements in Credential Validation.</t>
   </si>
   <si>
     <t xml:space="preserve">CRRC.05</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST ensure that credential recovery only applies to those credentials that are in a suspended state (i.e., revoked credentials cannot be recovered, they must be reissued).</t>
+    <t xml:space="preserve">The entity under assessment SHALL ensure that credential recovery only applies to those credentials that are in a suspended state (i.e., revoked credentials cannot be recovered, they SHALL be reissued).</t>
   </si>
   <si>
     <t xml:space="preserve">CRRC.06</t>
@@ -4541,7 +4454,7 @@
     <t xml:space="preserve">CRRV.01</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST have the ability to revoke the credential (for example, due to the expiry date having been exceeded or the detection of suspicious activity).</t>
+    <t xml:space="preserve">The entity under assessment SHALL have the ability to revoke the credential (for example, due to the expiry date having been exceeded or the detection of suspicious activity).</t>
   </si>
   <si>
     <t xml:space="preserve">CRRV.02</t>
@@ -4559,13 +4472,13 @@
     <t xml:space="preserve">CRRV.04</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST perform Identity Verification of the Holder making the credential revocation request.</t>
+    <t xml:space="preserve">The entity under assessment SHALL perform Identity Verification of the Holder making the credential revocation request.</t>
   </si>
   <si>
     <t xml:space="preserve">CRRV.05</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST ensure that credential revocation can only occur based on relevant policy, law, or regulation.</t>
+    <t xml:space="preserve">The entity under assessment SHALL ensure that credential revocation can only occur based on relevant policy, law, or regulation.</t>
   </si>
   <si>
     <t xml:space="preserve">CRRV.06</t>
@@ -4577,7 +4490,7 @@
     <t xml:space="preserve">CRRV.07</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST inform the Holder of the change in the credential status.</t>
+    <t xml:space="preserve">The entity under assessment SHALL inform the Holder of the change in the credential status.</t>
   </si>
   <si>
     <t xml:space="preserve">CRRV.08</t>
@@ -4598,7 +4511,7 @@
     <t xml:space="preserve">CODG.01</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST have a comprehensive Privacy Policy that:
+    <t xml:space="preserve">The entity under assessment SHALL have a comprehensive Privacy Policy that:
    ● provides a full description of its personal information handling practices;
    ● is easily accessible, simple to read, and updated as required; and
    ● is made available to clients and disseminated to internal personnel.</t>
@@ -4607,25 +4520,25 @@
     <t xml:space="preserve">CODG.02</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST periodically audit or review their personal information management practices (including its notice and consent management practices) to ensure that personal information is being handled in the way described by its Privacy Policy.</t>
+    <t xml:space="preserve">The entity under assessment SHALL periodically audit or review their personal information management practices (including its notice and consent management practices) to ensure that personal information is being handled in the way described by its Privacy Policy.</t>
   </si>
   <si>
     <t xml:space="preserve">CODG.03</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST have a Privacy Management Program in place to ensure legal compliance including the implementation of privacy policies, practices, controls, and assessment tools.</t>
+    <t xml:space="preserve">The entity under assessment SHALL have a Privacy Management Program in place to ensure legal compliance including the implementation of privacy policies, practices, controls, and assessment tools.</t>
   </si>
   <si>
     <t xml:space="preserve">CODG.04</t>
   </si>
   <si>
-    <t xml:space="preserve">As part of its Privacy Management Program, the entity under assessment MUST have processes to manage personal information breaches, which includes reporting, containment, remediation, and prevention steps.</t>
+    <t xml:space="preserve">As part of its Privacy Management Program, the entity under assessment SHALL have processes to manage personal information breaches, which includes reporting, containment, remediation, and prevention steps.</t>
   </si>
   <si>
     <t xml:space="preserve">CODG.05</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST have a Privacy Officer or similar position in place who is responsible for overseeing the Privacy Management Program and any internal audits or reviews of personal information handling practices (including those related to the provision of notice and the obtaining of consent).</t>
+    <t xml:space="preserve">The entity under assessment SHALL have a Privacy Officer or similar position in place who is responsible for overseeing the Privacy Management Program and any internal audits or reviews of personal information handling practices (including those related to the provision of notice and the obtaining of consent).</t>
   </si>
   <si>
     <t xml:space="preserve">CONF</t>
@@ -4667,13 +4580,13 @@
     <t xml:space="preserve">CONF.01</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST determine what information is required to be included in the consent notice statement based on all applicable legal, policy, and contractual requirements. This could include, for example:
+    <t xml:space="preserve">The entity under assessment SHALL determine what information is required to be included in the consent notice statement based on all applicable legal, policy, and contractual requirements. This could include, for example:
    ● the personal information about the Subject being requested;
    ● the purpose for which the personal information is being requested;
    ● the legal authority for collecting the personal information;
    ● if applicable, the period of time for which the personal information requested will be stored or used; and
    ● whether the request is for a one-time disclosure of the personal information or to allow ongoing disclosure for the same purpose (e.g., to allow the Subject to “broadcast” updates to their personal information, such as change of address).
-The entity under assessment MUST ensure that the information to be included in the consent notice statement is precisely defined. This could include, for example, the specific personal information to be shared and any necessary metadata.</t>
+The entity under assessment SHALL ensure that the information to be included in the consent notice statement is precisely defined. This could include, for example, the specific personal information to be shared and any necessary metadata.</t>
   </si>
   <si>
     <t xml:space="preserve">CONF.02</t>
@@ -4685,21 +4598,21 @@
     <t xml:space="preserve">CONF.03</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST ensure that the consent notice statement is formulated in a manner that enables the Subject to reasonably understand how their personal information will be collected, used, and/or disclosed. This includes providing the consent notice statement in a manner that is intelligible (using clear and plain language), concise, easily visible, and easily accessible.
-When it is not practical for the consent notice statement to include all the details pertaining to the request (e.g., the full terms and conditions, detailed metadata), the entity under assessment SHOULD provide the means to allow the Subject to review those details elsewhere. This MUST not be used as a means to make the consent notice statement less visible, transparent, or accessible.</t>
+    <t xml:space="preserve">The entity under assessment SHALL ensure that the consent notice statement is formulated in a manner that enables the Subject to reasonably understand how their personal information will be collected, used, and/or disclosed. This includes providing the consent notice statement in a manner that is intelligible (using clear and plain language), concise, easily visible, and easily accessible.
+When it is not practical for the consent notice statement to include all the details pertaining to the request (e.g., the full terms and conditions, detailed metadata), the entity under assessment SHOULD provide the means to allow the Subject to review those details elsewhere. This SHALL not be used as a means to make the consent notice statement less visible, transparent, or accessible.</t>
   </si>
   <si>
     <t xml:space="preserve">CONF.04</t>
   </si>
   <si>
-    <t xml:space="preserve">If the consent notice statement includes requests for a consent decison from multiple entities, then the entity under assessment MUST ensure that the consent notice statement is formulated such that the consent notice statement can be split up into the parts pertaining to each entity so that each entity only receives the evidence of the consent decision relevant to them.</t>
+    <t xml:space="preserve">If the consent notice statement includes requests for a consent decison from multiple entities, then the entity under assessment SHALL ensure that the consent notice statement is formulated such that the consent notice statement can be split up into the parts pertaining to each entity so that each entity only receives the evidence of the consent decision relevant to them.</t>
   </si>
   <si>
     <t xml:space="preserve">CONF.05</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST ensure that a new consent notice statement is provided to a Subject when the entity under assessment decides to use or disclose personal information that it has already collected from the Subject for a new purpose (i.e., a purpose that is not consistent with the purpose(s) provided in the original consent notice statement).
-The entity under assessment MUST ensure that the new consent notice statement:
+    <t xml:space="preserve">The entity under assessment SHALL ensure that a new consent notice statement is provided to a Subject when the entity under assessment decides to use or disclose personal information that it has already collected from the Subject for a new purpose (i.e., a purpose that is not consistent with the purpose(s) provided in the original consent notice statement).
+The entity under assessment SHALL ensure that the new consent notice statement:
    ● identifies the new purpose(s) and the specific personal information that will be used or disclosed for the new purpose(s);
    ● includes other applicable information that may be required; and,
    ● requests the Subject’s consent to use or disclose the personal information for the new purpose(s).</t>
@@ -4769,13 +4682,13 @@
     <t xml:space="preserve">CONP.01</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST present the consent notice statement to the person providing the consent in a manner that is clear and user friendly.</t>
+    <t xml:space="preserve">The entity under assessment SHALL present the consent notice statement to the person providing the consent in a manner that is clear and user friendly.</t>
   </si>
   <si>
     <t xml:space="preserve">CONP.02</t>
   </si>
   <si>
-    <t xml:space="preserve">If the consent notice statement discloses personal information then, before presenting the consent notice statement, the entity under assessment MUST verify the identity of the person providing the consent, to confirm that the person providing the consent is the Subject of the personal information, by executing the requirements in Identity Verification.</t>
+    <t xml:space="preserve">If the consent notice statement discloses personal information then, before presenting the consent notice statement, the entity under assessment SHALL verify the identity of the person providing the consent, to confirm that the person providing the consent is the Subject of the personal information, by executing the requirements in Identity Verification.</t>
   </si>
   <si>
     <t xml:space="preserve">CORQ</t>
@@ -4817,20 +4730,20 @@
     <t xml:space="preserve">CORQ.01</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST ensure the person providing the consent is the Subject of the personal information based on the requirements in Identity Verification.</t>
+    <t xml:space="preserve">The entity under assessment SHALL ensure the person providing the consent is the Subject of the personal information based on the requirements in Identity Verification.</t>
   </si>
   <si>
     <t xml:space="preserve">CORQ.02</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST ensure that the level of identity verification is sufficient for the sensitivity of personal data to be provided.</t>
+    <t xml:space="preserve">The entity under assessment SHALL ensure that the level of identity verification is sufficient for the sensitivity of personal data to be provided.</t>
   </si>
   <si>
     <t xml:space="preserve">CORQ.03</t>
   </si>
   <si>
-    <t xml:space="preserve">Before requesting consent from a Subject, the entity under assessment MUST determine whether the Subject can withdraw their consent at a later date or whether legal or contractual restrictions prevent or limit the withdrawal of consent.
-Where a Subject has the right to withdraw their consent at a later date, the entity under assessment MUST:
+    <t xml:space="preserve">Before requesting consent from a Subject, the entity under assessment SHALL determine whether the Subject can withdraw their consent at a later date or whether legal or contractual restrictions prevent or limit the withdrawal of consent.
+Where a Subject has the right to withdraw their consent at a later date, the entity under assessment SHALL:
    ● inform the Subject of this right (subject to reasonable notice and applicable conditions or restrictions) at the time the consent is requested;
    ● inform the Subject of how to exercise this right; and
    ● ensure that the process for withdrawing consent is as easy for the Subject as the process for providing consent.</t>
@@ -4839,7 +4752,7 @@
     <t xml:space="preserve">CORQ.04</t>
   </si>
   <si>
-    <t xml:space="preserve">If the Subject’s consent is requested as part of a consent notice statement which also concerns other matters, then the entity under assessment MUST present the request for consent in a manner that:
+    <t xml:space="preserve">If the Subject’s consent is requested as part of a consent notice statement which also concerns other matters, then the entity under assessment SHALL present the request for consent in a manner that:
    ● is clearly distinguishable from the other matters;
    ● is in an intelligible and easily accessible form; and
    ● uses clear and plain language.</t>
@@ -4848,20 +4761,20 @@
     <t xml:space="preserve">CORQ.05</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST ensure that the action required to be taken by the Subject to provide consent is clear and straightforward.
-If the Subject is offered a choice within the requested consent (e.g., to share a subset of the requested personal information), then the entity under assessment MUST ensure that the action required to make the choice is clear and straightforward.</t>
+    <t xml:space="preserve">The entity under assessment SHALL ensure that the action required to be taken by the Subject to provide consent is clear and straightforward.
+If the Subject is offered a choice within the requested consent (e.g., to share a subset of the requested personal information), then the entity under assessment SHALL ensure that the action required to make the choice is clear and straightforward.</t>
   </si>
   <si>
     <t xml:space="preserve">CORQ.06</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST ensure that the consent is specific, informed, and unambiguous.</t>
+    <t xml:space="preserve">The entity under assessment SHALL ensure that the consent is specific, informed, and unambiguous.</t>
   </si>
   <si>
     <t xml:space="preserve">CORQ.07</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST have processes in place that enable it to easily demonstrate that a Subject has consented to the collection, use, and/or disclosure of their personal information.</t>
+    <t xml:space="preserve">The entity under assessment SHALL have processes in place that enable it to easily demonstrate that a Subject has consented to the collection, use, and/or disclosure of their personal information.</t>
   </si>
   <si>
     <t xml:space="preserve">CORG</t>
@@ -4903,36 +4816,36 @@
     <t xml:space="preserve">CORG.01</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST collect and store the following evidence of the consent decision:
+    <t xml:space="preserve">The entity under assessment SHALL collect and store the following evidence of the consent decision:
    ● Sufficient information to identify the person who has given the consent; 
    ● The date, time, or other contextual information about when and how the consent decision was made;
    ● The version of the consent notice statement presented and the personal information requested;
-   ● The consent decision which MUST be one of accept or decline, for each consent choice presented; and
+   ● The consent decision which SHALL be one of accept or decline, for each consent choice presented; and
    ● If applicable, the expiration date/time of the consent decision.</t>
   </si>
   <si>
     <t xml:space="preserve">CORG.02</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST store the evidence of the consent decision uniquely (i.e., store the evidence of the consent decision for each consent given) and immutably, such that any update (including any change to the consent notice statement presented to the Subject) will result in a new record and therefore past records can be recovered. The entity under assessment MUST ensure that the storage of evidence of consent decisions complies with applicable legislation (e.g., in certain cases, data must be stored in Canada).</t>
+    <t xml:space="preserve">The entity under assessment SHALL store the evidence of the consent decision uniquely (i.e., store the evidence of the consent decision for each consent given) and immutably, such that any update (including any change to the consent notice statement presented to the Subject) will result in a new record and therefore past records can be recovered. The entity under assessment SHALL ensure that the storage of evidence of consent decisions complies with applicable legislation (e.g., in certain cases, data SHALL be stored in Canada).</t>
   </si>
   <si>
     <t xml:space="preserve">CORG.03</t>
   </si>
   <si>
-    <t xml:space="preserve">As per Canadian laws related to official language requirements, the entity under assessment MUST store each language variation of the consent notice statement.</t>
+    <t xml:space="preserve">As per Canadian laws related to official language requirements, the entity under assessment SHALL store each language variation of the consent notice statement.</t>
   </si>
   <si>
     <t xml:space="preserve">CORG.04</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST employ processes and procedures to prevent the loss of notice and consent decision records and to limit the impact of any data security violations, and in accordance with relevant law.</t>
+    <t xml:space="preserve">The entity under assessment SHALL employ processes and procedures to prevent the loss of notice and consent decision records and to limit the impact of any data security violations, and in accordance with relevant law.</t>
   </si>
   <si>
     <t xml:space="preserve">CORG.05</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST follow privacy-preserving practices when storing records of consent decisions. In this context, privacy-preserving practices refer to methods, approaches, or procedures designed to maintain the privacy of consent decision records.</t>
+    <t xml:space="preserve">The entity under assessment SHALL follow privacy-preserving practices when storing records of consent decisions. In this context, privacy-preserving practices refer to methods, approaches, or procedures designed to maintain the privacy of consent decision records.</t>
   </si>
   <si>
     <t xml:space="preserve">CORG.06</t>
@@ -4940,7 +4853,7 @@
   <si>
     <t xml:space="preserve">If the entity under assessment provides the evidence of the consent decision to another requesting entity: 
    ● The entity under assessment SHOULD inform the Subject of the identity of the other entity receiving the evidence of the consent decision; 
-   ● If the consent notice statement includes requests for a consent decison from multiple entities, the entity under assessment MUST split up the consent notice statement so that each entity only receives the evidence of the consent decision relevant to them.</t>
+   ● If the consent notice statement includes requests for a consent decison from multiple entities, the entity under assessment SHALL split up the consent notice statement so that each entity only receives the evidence of the consent decision relevant to them.</t>
   </si>
   <si>
     <t xml:space="preserve">CORE</t>
@@ -5004,19 +4917,19 @@
     <t xml:space="preserve">CORN.01</t>
   </si>
   <si>
-    <t xml:space="preserve">In order to extend the validity period of a “yes” consent decision, the entity under assessment MUST execute the requirements in Consent Notice Formulation, Consent Notice Presentation, Consent Request, and Consent Registration. The entity under assessment MUST store the resulting updated consent decision.</t>
+    <t xml:space="preserve">In order to extend the validity period of a “yes” consent decision, the entity under assessment SHALL execute the requirements in Consent Notice Formulation, Consent Notice Presentation, Consent Request, and Consent Registration. The entity under assessment SHALL store the resulting updated consent decision.</t>
   </si>
   <si>
     <t xml:space="preserve">CORN.02</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST record the following consent renewal information: the effective date of renewal and the initiating party for the renewal.</t>
+    <t xml:space="preserve">The entity under assessment SHALL record the following consent renewal information: the effective date of renewal and the initiating party for the renewal.</t>
   </si>
   <si>
     <t xml:space="preserve">CORN.03</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST make available consent renewal information to the Subject and any Verifier.</t>
+    <t xml:space="preserve">The entity under assessment SHALL make available consent renewal information to the Subject and any Verifier.</t>
   </si>
   <si>
     <t xml:space="preserve">COEX</t>
@@ -5034,19 +4947,19 @@
     <t xml:space="preserve">COEX.01</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST ensure that a consent decision expires when the expiration date of the consent decision has passed. </t>
+    <t xml:space="preserve">The entity under assessment SHALL ensure that a consent decision expires when the expiration date of the consent decision has passed. </t>
   </si>
   <si>
     <t xml:space="preserve">COEX.02</t>
   </si>
   <si>
-    <t xml:space="preserve">Unless the collection, use, or disclosure is permitted without consent, the entity under assessment MUST stop collecting, using, or disclosing the personal information specified in the consent decision and MUST inform any entity to whom the the evidence of the consent decision was sent of the expired consent decision.</t>
+    <t xml:space="preserve">Unless the collection, use, or disclosure is permitted without consent, the entity under assessment SHALL stop collecting, using, or disclosing the personal information specified in the consent decision and SHALL inform any entity to whom the the evidence of the consent decision was sent of the expired consent decision.</t>
   </si>
   <si>
     <t xml:space="preserve">COEX.03</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST record the following consent expiry information: the effective date of expiry and the initiating party for the expiry.</t>
+    <t xml:space="preserve">The entity under assessment SHALL record the following consent expiry information: the effective date of expiry and the initiating party for the expiry.</t>
   </si>
   <si>
     <t xml:space="preserve">COEX.04</t>
@@ -5071,7 +4984,7 @@
     <t xml:space="preserve">CORV.01</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST revoke a consent decision when either:
+    <t xml:space="preserve">The entity under assessment SHALL revoke a consent decision when either:
     ● the Subject withdraws the consent; or
     ● the entity under assessment determines that the consent was not legitimate or lawful, for example, if a fraudulent activity, data breach, or unauthorised access is determined.</t>
   </si>
@@ -5080,64 +4993,34 @@
   </si>
   <si>
     <t xml:space="preserve">If a Subject notifies the entity under assessment that they wish to withdraw the consent given and there are no legal or contractual restrictions preventing the Subject from withdrawing consent, then the entity under assessment:
-    ● MUST inform the Subject of the implications of such withdrawal; 
-    ● MUST NOT prohibit the Subject from withdrawing consent; and
-    ● MUST ensure that the action required to withdraw the consent is clear, explicit, and straightforward.</t>
+    ● SHALL inform the Subject of the implications of such withdrawal; 
+    ● SHALL NOT prohibit the Subject from withdrawing consent; and
+    ● SHALL ensure that the action required to withdraw the consent is clear, explicit, and straightforward.</t>
   </si>
   <si>
     <t xml:space="preserve">CORV.03</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">If it is determined that the consent was not legitimate or lawful, then the entity under assessment MUST revoke the consent decision.
-The entity under assessment MUST inform the Subject of the revoked consent decision (if appropriate). </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Note</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">: In the case of identity theft where the Subject is compromised it may not be appropriate to inform the Subject of the revoked consent decision. In the interest of protecting identity information from abuse and privacy breaches, revoking consent in such circumstances MUST be done with great care. The entity under assessment MUST ensure that it has processes in place to prevent erroneous or malicious consent revocation.</t>
-    </r>
+    <t xml:space="preserve">If it is determined that the consent was not legitimate or lawful, then the entity under assessment SHALL revoke the consent decision.
+The entity under assessment SHALL inform the Subject of the revoked consent decision (if appropriate). Note: In the case of identity theft where the Subject is compromised it may not be appropriate to inform the Subject of the revoked consent decision. In the interest of protecting identity information from abuse and privacy breaches, revoking consent in such circumstances SHALL be done with great care. The entity under assessment SHALL ensure that it has processes in place to prevent erroneous or malicious consent revocation.</t>
   </si>
   <si>
     <t xml:space="preserve">CORV.04</t>
   </si>
   <si>
-    <t xml:space="preserve">Unless the collection, use, or disclosure is permitted without consent, the entity under assessment MUST stop collecting, using, or disclosing the personal information specified in the consent decision and MUST inform any entity to whom the the evidence of the consent decision was sent of the revoked consent decision.</t>
+    <t xml:space="preserve">Unless the collection, use, or disclosure is permitted without consent, the entity under assessment SHALL stop collecting, using, or disclosing the personal information specified in the consent decision and SHALL inform any entity to whom the the evidence of the consent decision was sent of the revoked consent decision.</t>
   </si>
   <si>
     <t xml:space="preserve">CORV.05</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST record the following consent revocation information: the effective date of revocation, the reason for revocation, and the initiating party for the revocation.</t>
+    <t xml:space="preserve">The entity under assessment SHALL record the following consent revocation information: the effective date of revocation, the reason for revocation, and the initiating party for the revocation.</t>
   </si>
   <si>
     <t xml:space="preserve">CORV.06</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST make available consent revocation information to the Subject and any Verifier.</t>
+    <t xml:space="preserve">The entity under assessment SHALL make available consent revocation information to the Subject and any Verifier.</t>
   </si>
   <si>
     <t xml:space="preserve">SIDG</t>
@@ -5194,25 +5077,25 @@
     <t xml:space="preserve">SICR.01</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST ensure that the entity signing the data can be associated with the electronic data being signed.</t>
+    <t xml:space="preserve">The entity under assessment SHALL ensure that the entity signing the data can be associated with the electronic data being signed.</t>
   </si>
   <si>
     <t xml:space="preserve">SICR.02</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST ensure that it is clear that the entity intended to sign the electronic record.</t>
+    <t xml:space="preserve">The entity under assessment SHALL ensure that it is clear that the entity intended to sign the electronic record.</t>
   </si>
   <si>
     <t xml:space="preserve">SICR.03</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST ensure that the reason or purpose for signing the electronic data is conveyed in some way (this may be evident from the content of the electronic data being signed).</t>
+    <t xml:space="preserve">The entity under assessment SHALL ensure that the reason or purpose for signing the electronic data is conveyed in some way (this may be evident from the content of the electronic data being signed).</t>
   </si>
   <si>
     <t xml:space="preserve">SICR.04</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST ensure that the data integrity of the signed transaction is maintained over time including the original electronic data being signed, the electronic signature itself, and any supporting information that may be necessary.</t>
+    <t xml:space="preserve">The entity under assessment SHALL ensure that the data integrity of the signed transaction is maintained over time including the original electronic data being signed, the electronic signature itself, and any supporting information that may be necessary.</t>
   </si>
   <si>
     <t xml:space="preserve">SICR.05</t>
@@ -5221,25 +5104,25 @@
     <t xml:space="preserve">SES</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST ensure that the electronic data has been signed by the entity who is identified in, or can be identified through, a digital signature certificate.</t>
+    <t xml:space="preserve">The entity under assessment SHALL ensure that the electronic data has been signed by the entity who is identified in, or can be identified through, a digital signature certificate.</t>
   </si>
   <si>
     <t xml:space="preserve">SICR.06</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST ensure that specific asymmetric algorithms are used.</t>
+    <t xml:space="preserve">The entity under assessment SHALL ensure that specific asymmetric algorithms are used.</t>
   </si>
   <si>
     <t xml:space="preserve">SICR.07</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST ensure that the issuing certification authority (CA) is recognized by a competent authority.</t>
+    <t xml:space="preserve">The entity under assessment SHALL ensure that the issuing certification authority (CA) is recognized by a competent authority.</t>
   </si>
   <si>
     <t xml:space="preserve">SICR.08</t>
   </si>
   <si>
-    <t xml:space="preserve">The entity under assessment MUST verify that the issuing certification authority (CA) has the capacity to issue digital signature certificates in a secure and reliable manner.</t>
+    <t xml:space="preserve">The entity under assessment SHALL verify that the issuing certification authority (CA) has the capacity to issue digital signature certificates in a secure and reliable manner.</t>
   </si>
   <si>
     <t xml:space="preserve">SICH</t>
@@ -6405,7 +6288,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="2" borderId="3" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="3" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -7405,11 +7288,11 @@
   </sheetPr>
   <dimension ref="A1:V55"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="118.33"/>
@@ -7868,8 +7751,8 @@
     <mergeCell ref="A25:A33"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -7890,7 +7773,7 @@
       <selection pane="bottomLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.66"/>
@@ -10256,8 +10139,8 @@
     <hyperlink ref="D24" r:id="rId21" display="https://www.itu.int/rec/T-REC-X.1255-201309-I"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -10276,14 +10159,14 @@
       <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="31.31"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -10302,7 +10185,7 @@
       <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="42.87"/>
@@ -10375,7 +10258,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -10391,10 +10274,10 @@
   <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
+      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="47.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="55" width="14.88"/>
@@ -10778,14 +10661,14 @@
     <mergeCell ref="C1:D1"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H4:H9 H11:H16 H18:H23 H25:H29" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H4:H9 H11:H16 H18:H23 H25:H29" type="list">
       <formula1>"PENDING,CONFORM,NON-CONFORM,NOT APPLICABLE,OUT OF SCOPE,COMMENT"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -10802,12 +10685,12 @@
   <dimension ref="A1:I1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="2" topLeftCell="A454" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B43" activeCellId="0" sqref="B43"/>
+      <selection pane="bottomLeft" activeCell="F465" activeCellId="0" sqref="F465"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="61.69"/>
@@ -19156,22 +19039,22 @@
     <mergeCell ref="C460:I460"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H6" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H6" type="list">
       <formula1>"PENDING,CONFORM,NON-CONFORM,NOT APPLICABLE,OUT OF SCOPE,"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H7:H8" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H7:H8" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H4 H24 H40 H47 H57 H69 H80 H86 H101 H109 H115 H129 H138 H152 H161 H169 H179 H188 H194 H206 H213 H218 H228 H243 H255 H268 H281 H292 H301 H308 H315 H322 H336 H348 H361 H371 H380 H387 H399 H410 H416 H424 H433 H444 H449" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H4 H24 H40 H47 H57 H69 H80 H86 H101 H109 H115 H129 H138 H152 H161 H169 H179 H188 H194 H206 H213 H218 H228 H243 H255 H268 H281 H292 H301 H308 H315 H322 H336 H348 H361 H371 H380 H387 H399 H410 H416 H424 H433 H444 H449" type="list">
       <formula1>"PENDING,CONFORM,NON-CONFORM,NOT APPLICABLE,OUT OF SCOPE,COMMENT"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -19187,11 +19070,11 @@
   </sheetPr>
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="48.46"/>
@@ -19578,7 +19461,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -19594,11 +19477,11 @@
   </sheetPr>
   <dimension ref="A1:Z1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B28" activeCellId="0" sqref="B28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="44.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="56.66"/>
@@ -21203,8 +21086,8 @@
     <mergeCell ref="A60:A61"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -21225,7 +21108,7 @@
       <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.66"/>
@@ -24345,8 +24228,8 @@
     <row r="1000" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -24365,7 +24248,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="173.33"/>
@@ -25597,8 +25480,8 @@
     <mergeCell ref="A29:B29"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -25619,7 +25502,7 @@
       <selection pane="bottomLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="236" width="14.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="16.67"/>
@@ -27359,8 +27242,8 @@
     <row r="999" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>